<commit_message>
Update TMT matrix math files
</commit_message>
<xml_diff>
--- a/Docs/TMT11plex_Calculations_Lots_A37725_TB265130.xlsx
+++ b/Docs/TMT11plex_Calculations_Lots_A37725_TB265130.xlsx
@@ -151,7 +151,7 @@
   <numFmts count="3">
     <numFmt numFmtId="164" formatCode="0.000"/>
     <numFmt numFmtId="165" formatCode="0.0%"/>
-    <numFmt numFmtId="171" formatCode="0.0000"/>
+    <numFmt numFmtId="166" formatCode="0.0000"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -213,9 +213,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
@@ -227,13 +224,16 @@
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="171" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="171" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -518,8 +518,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:AG40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="R1" workbookViewId="0">
-      <selection activeCell="W16" sqref="W16"/>
+    <sheetView tabSelected="1" topLeftCell="S10" workbookViewId="0">
+      <selection activeCell="V16" sqref="V16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -539,41 +539,41 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:33" x14ac:dyDescent="0.3">
-      <c r="C2" s="10" t="s">
+      <c r="C2" s="19" t="s">
         <v>35</v>
       </c>
-      <c r="D2" s="10"/>
-      <c r="E2" s="10"/>
-      <c r="F2" s="10"/>
-      <c r="G2" s="10"/>
+      <c r="D2" s="19"/>
+      <c r="E2" s="19"/>
+      <c r="F2" s="19"/>
+      <c r="G2" s="19"/>
       <c r="H2" s="8"/>
-      <c r="I2" s="10" t="s">
+      <c r="I2" s="19" t="s">
         <v>20</v>
       </c>
-      <c r="J2" s="10"/>
-      <c r="K2" s="10"/>
-      <c r="L2" s="10"/>
-      <c r="M2" s="10"/>
-      <c r="O2" s="10" t="s">
+      <c r="J2" s="19"/>
+      <c r="K2" s="19"/>
+      <c r="L2" s="19"/>
+      <c r="M2" s="19"/>
+      <c r="O2" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="P2" s="10"/>
-      <c r="Q2" s="10"/>
-      <c r="R2" s="10"/>
-      <c r="S2" s="10"/>
-      <c r="W2" s="10" t="s">
+      <c r="P2" s="19"/>
+      <c r="Q2" s="19"/>
+      <c r="R2" s="19"/>
+      <c r="S2" s="19"/>
+      <c r="W2" s="19" t="s">
         <v>37</v>
       </c>
-      <c r="X2" s="10"/>
-      <c r="Y2" s="10"/>
-      <c r="Z2" s="10"/>
-      <c r="AA2" s="10"/>
-      <c r="AB2" s="10"/>
-      <c r="AC2" s="10"/>
-      <c r="AD2" s="10"/>
-      <c r="AE2" s="10"/>
-      <c r="AF2" s="10"/>
-      <c r="AG2" s="10"/>
+      <c r="X2" s="19"/>
+      <c r="Y2" s="19"/>
+      <c r="Z2" s="19"/>
+      <c r="AA2" s="19"/>
+      <c r="AB2" s="19"/>
+      <c r="AC2" s="19"/>
+      <c r="AD2" s="19"/>
+      <c r="AE2" s="19"/>
+      <c r="AF2" s="19"/>
+      <c r="AG2" s="19"/>
     </row>
     <row r="3" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A3" s="8" t="s">
@@ -671,10 +671,10 @@
       </c>
     </row>
     <row r="4" spans="1:33" x14ac:dyDescent="0.3">
-      <c r="A4" s="18" t="s">
+      <c r="A4" s="17" t="s">
         <v>21</v>
       </c>
-      <c r="B4" s="19">
+      <c r="B4" s="18">
         <v>126.127726</v>
       </c>
       <c r="C4" s="8">
@@ -683,58 +683,58 @@
       <c r="D4" s="8">
         <v>0</v>
       </c>
-      <c r="E4" s="14">
+      <c r="E4" s="13">
         <v>1</v>
       </c>
-      <c r="F4" s="13">
+      <c r="F4" s="12">
         <v>8.2000000000000003E-2</v>
       </c>
-      <c r="G4" s="13">
+      <c r="G4" s="12">
         <v>4.0000000000000001E-3</v>
       </c>
       <c r="H4" s="4"/>
-      <c r="I4" s="13">
+      <c r="I4" s="12">
         <f>C4/SUM($C4:$G4)</f>
         <v>0</v>
       </c>
-      <c r="J4" s="13">
+      <c r="J4" s="12">
         <f t="shared" ref="J4:M4" si="2">D4/SUM($C4:$G4)</f>
         <v>0</v>
       </c>
-      <c r="K4" s="13">
+      <c r="K4" s="12">
         <f t="shared" si="2"/>
         <v>0.92081031307550643</v>
       </c>
-      <c r="L4" s="13">
+      <c r="L4" s="12">
         <f t="shared" si="2"/>
         <v>7.550644567219153E-2</v>
       </c>
-      <c r="M4" s="13">
+      <c r="M4" s="12">
         <f t="shared" si="2"/>
         <v>3.6832412523020255E-3</v>
       </c>
       <c r="N4" s="4"/>
-      <c r="O4" s="15">
+      <c r="O4" s="14">
         <f>I4</f>
         <v>0</v>
       </c>
-      <c r="P4" s="15">
+      <c r="P4" s="14">
         <f t="shared" ref="P4:S14" si="3">J4</f>
         <v>0</v>
       </c>
-      <c r="Q4" s="16">
+      <c r="Q4" s="15">
         <f t="shared" si="3"/>
         <v>0.92081031307550643</v>
       </c>
-      <c r="R4" s="16">
+      <c r="R4" s="15">
         <f t="shared" ref="R4" si="4">L4</f>
         <v>7.550644567219153E-2</v>
       </c>
-      <c r="S4" s="16">
+      <c r="S4" s="15">
         <f t="shared" ref="S4" si="5">M4</f>
         <v>3.6832412523020255E-3</v>
       </c>
-      <c r="V4" s="15">
+      <c r="V4" s="14">
         <v>0</v>
       </c>
       <c r="W4" s="2">
@@ -759,69 +759,69 @@
       <c r="AG4" s="2"/>
     </row>
     <row r="5" spans="1:33" x14ac:dyDescent="0.3">
-      <c r="A5" s="18" t="s">
+      <c r="A5" s="17" t="s">
         <v>22</v>
       </c>
-      <c r="B5" s="19">
+      <c r="B5" s="18">
         <v>127.12476100000001</v>
       </c>
       <c r="C5" s="8">
         <v>0</v>
       </c>
-      <c r="D5" s="13">
+      <c r="D5" s="12">
         <v>1E-3</v>
       </c>
-      <c r="E5" s="14">
+      <c r="E5" s="13">
         <v>1</v>
       </c>
-      <c r="F5" s="13">
+      <c r="F5" s="12">
         <v>7.9000000000000001E-2</v>
       </c>
       <c r="G5" s="8">
         <v>0</v>
       </c>
-      <c r="I5" s="13">
+      <c r="I5" s="12">
         <f t="shared" ref="I5:I14" si="6">C5/SUM($C5:$G5)</f>
         <v>0</v>
       </c>
-      <c r="J5" s="13">
+      <c r="J5" s="12">
         <f t="shared" ref="J5:J14" si="7">D5/SUM($C5:$G5)</f>
         <v>9.2592592592592607E-4</v>
       </c>
-      <c r="K5" s="13">
+      <c r="K5" s="12">
         <f t="shared" ref="K5:K14" si="8">E5/SUM($C5:$G5)</f>
         <v>0.92592592592592604</v>
       </c>
-      <c r="L5" s="13">
+      <c r="L5" s="12">
         <f t="shared" ref="L5:L14" si="9">F5/SUM($C5:$G5)</f>
         <v>7.3148148148148157E-2</v>
       </c>
-      <c r="M5" s="13">
+      <c r="M5" s="12">
         <f t="shared" ref="M5:M14" si="10">G5/SUM($C5:$G5)</f>
         <v>0</v>
       </c>
       <c r="N5" s="4"/>
-      <c r="O5" s="15">
+      <c r="O5" s="14">
         <f t="shared" ref="O5:O14" si="11">I5</f>
         <v>0</v>
       </c>
-      <c r="P5" s="16">
+      <c r="P5" s="15">
         <f t="shared" si="3"/>
         <v>9.2592592592592607E-4</v>
       </c>
-      <c r="Q5" s="16">
+      <c r="Q5" s="15">
         <f t="shared" si="3"/>
         <v>0.92592592592592604</v>
       </c>
-      <c r="R5" s="16">
+      <c r="R5" s="15">
         <f t="shared" si="3"/>
         <v>7.3148148148148157E-2</v>
       </c>
-      <c r="S5" s="15">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="V5" s="15">
+      <c r="S5" s="14">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="V5" s="14">
         <v>1</v>
       </c>
       <c r="W5" s="2"/>
@@ -846,69 +846,69 @@
       <c r="AG5" s="2"/>
     </row>
     <row r="6" spans="1:33" x14ac:dyDescent="0.3">
-      <c r="A6" s="18" t="s">
+      <c r="A6" s="17" t="s">
         <v>23</v>
       </c>
-      <c r="B6" s="19">
+      <c r="B6" s="18">
         <v>127.13108099999999</v>
       </c>
       <c r="C6" s="8">
         <v>0</v>
       </c>
-      <c r="D6" s="13">
+      <c r="D6" s="12">
         <v>5.0000000000000001E-3</v>
       </c>
-      <c r="E6" s="14">
+      <c r="E6" s="13">
         <v>1</v>
       </c>
-      <c r="F6" s="13">
+      <c r="F6" s="12">
         <v>6.3E-2</v>
       </c>
       <c r="G6" s="8">
         <v>0</v>
       </c>
-      <c r="I6" s="13">
+      <c r="I6" s="12">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
-      <c r="J6" s="13">
+      <c r="J6" s="12">
         <f t="shared" si="7"/>
         <v>4.6816479400749074E-3</v>
       </c>
-      <c r="K6" s="13">
+      <c r="K6" s="12">
         <f t="shared" si="8"/>
         <v>0.93632958801498145</v>
       </c>
-      <c r="L6" s="13">
+      <c r="L6" s="12">
         <f t="shared" si="9"/>
         <v>5.8988764044943832E-2</v>
       </c>
-      <c r="M6" s="13">
+      <c r="M6" s="12">
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="N6" s="4"/>
-      <c r="O6" s="15">
+      <c r="O6" s="14">
         <f t="shared" si="11"/>
         <v>0</v>
       </c>
-      <c r="P6" s="16">
+      <c r="P6" s="15">
         <f t="shared" si="3"/>
         <v>4.6816479400749074E-3</v>
       </c>
-      <c r="Q6" s="16">
+      <c r="Q6" s="15">
         <f t="shared" si="3"/>
         <v>0.93632958801498145</v>
       </c>
-      <c r="R6" s="16">
+      <c r="R6" s="15">
         <f t="shared" si="3"/>
         <v>5.8988764044943832E-2</v>
       </c>
-      <c r="S6" s="15">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="V6" s="15">
+      <c r="S6" s="14">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="V6" s="14">
         <v>2</v>
       </c>
       <c r="W6" s="2">
@@ -936,69 +936,69 @@
       <c r="AG6" s="2"/>
     </row>
     <row r="7" spans="1:33" x14ac:dyDescent="0.3">
-      <c r="A7" s="18" t="s">
+      <c r="A7" s="17" t="s">
         <v>24</v>
       </c>
-      <c r="B7" s="19">
+      <c r="B7" s="18">
         <v>128.12811600000001</v>
       </c>
       <c r="C7" s="8">
         <v>0</v>
       </c>
-      <c r="D7" s="13">
+      <c r="D7" s="12">
         <v>7.0000000000000001E-3</v>
       </c>
-      <c r="E7" s="14">
+      <c r="E7" s="13">
         <v>1</v>
       </c>
-      <c r="F7" s="13">
+      <c r="F7" s="12">
         <v>5.7000000000000002E-2</v>
       </c>
       <c r="G7" s="8">
         <v>0</v>
       </c>
-      <c r="I7" s="13">
+      <c r="I7" s="12">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
-      <c r="J7" s="13">
+      <c r="J7" s="12">
         <f t="shared" si="7"/>
         <v>6.578947368421054E-3</v>
       </c>
-      <c r="K7" s="13">
+      <c r="K7" s="12">
         <f t="shared" si="8"/>
         <v>0.93984962406015049</v>
       </c>
-      <c r="L7" s="13">
+      <c r="L7" s="12">
         <f t="shared" si="9"/>
         <v>5.3571428571428582E-2</v>
       </c>
-      <c r="M7" s="13">
+      <c r="M7" s="12">
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="N7" s="4"/>
-      <c r="O7" s="15">
+      <c r="O7" s="14">
         <f t="shared" si="11"/>
         <v>0</v>
       </c>
-      <c r="P7" s="16">
+      <c r="P7" s="15">
         <f t="shared" si="3"/>
         <v>6.578947368421054E-3</v>
       </c>
-      <c r="Q7" s="16">
+      <c r="Q7" s="15">
         <f t="shared" si="3"/>
         <v>0.93984962406015049</v>
       </c>
-      <c r="R7" s="16">
+      <c r="R7" s="15">
         <f t="shared" si="3"/>
         <v>5.3571428571428582E-2</v>
       </c>
-      <c r="S7" s="15">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="V7" s="15">
+      <c r="S7" s="14">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="V7" s="14">
         <v>3</v>
       </c>
       <c r="W7" s="2"/>
@@ -1026,69 +1026,69 @@
       <c r="AG7" s="2"/>
     </row>
     <row r="8" spans="1:33" x14ac:dyDescent="0.3">
-      <c r="A8" s="18" t="s">
+      <c r="A8" s="17" t="s">
         <v>25</v>
       </c>
-      <c r="B8" s="19">
+      <c r="B8" s="18">
         <v>128.13443599999999</v>
       </c>
-      <c r="C8" s="14">
+      <c r="C8" s="13">
         <v>2E-3</v>
       </c>
-      <c r="D8" s="13">
+      <c r="D8" s="12">
         <v>1.6E-2</v>
       </c>
-      <c r="E8" s="14">
+      <c r="E8" s="13">
         <v>1</v>
       </c>
-      <c r="F8" s="13">
+      <c r="F8" s="12">
         <v>0.06</v>
       </c>
       <c r="G8" s="8">
         <v>0</v>
       </c>
-      <c r="I8" s="13">
+      <c r="I8" s="12">
         <f t="shared" si="6"/>
         <v>1.8552875695732837E-3</v>
       </c>
-      <c r="J8" s="13">
+      <c r="J8" s="12">
         <f t="shared" si="7"/>
         <v>1.4842300556586269E-2</v>
       </c>
-      <c r="K8" s="13">
+      <c r="K8" s="12">
         <f t="shared" si="8"/>
         <v>0.92764378478664189</v>
       </c>
-      <c r="L8" s="13">
+      <c r="L8" s="12">
         <f t="shared" si="9"/>
         <v>5.5658627087198508E-2</v>
       </c>
-      <c r="M8" s="13">
+      <c r="M8" s="12">
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="N8" s="4"/>
-      <c r="O8" s="16">
+      <c r="O8" s="15">
         <f t="shared" si="11"/>
         <v>1.8552875695732837E-3</v>
       </c>
-      <c r="P8" s="16">
+      <c r="P8" s="15">
         <f t="shared" si="3"/>
         <v>1.4842300556586269E-2</v>
       </c>
-      <c r="Q8" s="16">
+      <c r="Q8" s="15">
         <f t="shared" si="3"/>
         <v>0.92764378478664189</v>
       </c>
-      <c r="R8" s="16">
+      <c r="R8" s="15">
         <f t="shared" si="3"/>
         <v>5.5658627087198508E-2</v>
       </c>
-      <c r="S8" s="15">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="V8" s="15">
+      <c r="S8" s="14">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="V8" s="14">
         <v>4</v>
       </c>
       <c r="W8" s="2">
@@ -1119,69 +1119,69 @@
       <c r="AG8" s="2"/>
     </row>
     <row r="9" spans="1:33" x14ac:dyDescent="0.3">
-      <c r="A9" s="18" t="s">
+      <c r="A9" s="17" t="s">
         <v>26</v>
       </c>
-      <c r="B9" s="19">
+      <c r="B9" s="18">
         <v>129.131471</v>
       </c>
       <c r="C9" s="8">
         <v>0</v>
       </c>
-      <c r="D9" s="13">
+      <c r="D9" s="12">
         <v>2.5000000000000001E-2</v>
       </c>
-      <c r="E9" s="14">
+      <c r="E9" s="13">
         <v>1</v>
       </c>
-      <c r="F9" s="13">
+      <c r="F9" s="12">
         <v>0.05</v>
       </c>
       <c r="G9" s="8">
         <v>0</v>
       </c>
-      <c r="I9" s="13">
+      <c r="I9" s="12">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
-      <c r="J9" s="13">
+      <c r="J9" s="12">
         <f t="shared" si="7"/>
         <v>2.3255813953488375E-2</v>
       </c>
-      <c r="K9" s="13">
+      <c r="K9" s="12">
         <f t="shared" si="8"/>
         <v>0.93023255813953487</v>
       </c>
-      <c r="L9" s="13">
+      <c r="L9" s="12">
         <f t="shared" si="9"/>
         <v>4.651162790697675E-2</v>
       </c>
-      <c r="M9" s="13">
+      <c r="M9" s="12">
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="N9" s="4"/>
-      <c r="O9" s="15">
+      <c r="O9" s="14">
         <f t="shared" si="11"/>
         <v>0</v>
       </c>
-      <c r="P9" s="16">
+      <c r="P9" s="15">
         <f t="shared" si="3"/>
         <v>2.3255813953488375E-2</v>
       </c>
-      <c r="Q9" s="16">
+      <c r="Q9" s="15">
         <f t="shared" si="3"/>
         <v>0.93023255813953487</v>
       </c>
-      <c r="R9" s="16">
+      <c r="R9" s="15">
         <f t="shared" si="3"/>
         <v>4.651162790697675E-2</v>
       </c>
-      <c r="S9" s="15">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="V9" s="15">
+      <c r="S9" s="14">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="V9" s="14">
         <v>5</v>
       </c>
       <c r="W9" s="2"/>
@@ -1212,69 +1212,69 @@
       <c r="AG9" s="2"/>
     </row>
     <row r="10" spans="1:33" x14ac:dyDescent="0.3">
-      <c r="A10" s="18" t="s">
+      <c r="A10" s="17" t="s">
         <v>27</v>
       </c>
-      <c r="B10" s="19">
+      <c r="B10" s="18">
         <v>129.13779</v>
       </c>
       <c r="C10" s="8">
         <v>0</v>
       </c>
-      <c r="D10" s="13">
+      <c r="D10" s="12">
         <v>2.3E-2</v>
       </c>
-      <c r="E10" s="14">
+      <c r="E10" s="13">
         <v>1</v>
       </c>
-      <c r="F10" s="13">
+      <c r="F10" s="12">
         <v>4.2999999999999997E-2</v>
       </c>
       <c r="G10" s="8">
         <v>0</v>
       </c>
-      <c r="I10" s="13">
+      <c r="I10" s="12">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
-      <c r="J10" s="13">
+      <c r="J10" s="12">
         <f t="shared" si="7"/>
         <v>2.1575984990619138E-2</v>
       </c>
-      <c r="K10" s="13">
+      <c r="K10" s="12">
         <f t="shared" si="8"/>
         <v>0.93808630393996262</v>
       </c>
-      <c r="L10" s="13">
+      <c r="L10" s="12">
         <f t="shared" si="9"/>
         <v>4.0337711069418386E-2</v>
       </c>
-      <c r="M10" s="13">
+      <c r="M10" s="12">
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="N10" s="4"/>
-      <c r="O10" s="15">
+      <c r="O10" s="14">
         <f t="shared" si="11"/>
         <v>0</v>
       </c>
-      <c r="P10" s="16">
+      <c r="P10" s="15">
         <f t="shared" si="3"/>
         <v>2.1575984990619138E-2</v>
       </c>
-      <c r="Q10" s="16">
+      <c r="Q10" s="15">
         <f t="shared" si="3"/>
         <v>0.93808630393996262</v>
       </c>
-      <c r="R10" s="16">
+      <c r="R10" s="15">
         <f t="shared" si="3"/>
         <v>4.0337711069418386E-2</v>
       </c>
-      <c r="S10" s="15">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="V10" s="15">
+      <c r="S10" s="14">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="V10" s="14">
         <v>6</v>
       </c>
       <c r="W10" s="2"/>
@@ -1305,69 +1305,69 @@
       </c>
     </row>
     <row r="11" spans="1:33" x14ac:dyDescent="0.3">
-      <c r="A11" s="18" t="s">
+      <c r="A11" s="17" t="s">
         <v>28</v>
       </c>
-      <c r="B11" s="19">
+      <c r="B11" s="18">
         <v>130.13482500000001</v>
       </c>
       <c r="C11" s="8">
         <v>0</v>
       </c>
-      <c r="D11" s="13">
+      <c r="D11" s="12">
         <v>2.7E-2</v>
       </c>
-      <c r="E11" s="14">
+      <c r="E11" s="13">
         <v>1</v>
       </c>
-      <c r="F11" s="13">
+      <c r="F11" s="12">
         <v>3.9E-2</v>
       </c>
       <c r="G11" s="8">
         <v>0</v>
       </c>
-      <c r="I11" s="13">
+      <c r="I11" s="12">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
-      <c r="J11" s="13">
+      <c r="J11" s="12">
         <f t="shared" si="7"/>
         <v>2.532833020637899E-2</v>
       </c>
-      <c r="K11" s="13">
+      <c r="K11" s="12">
         <f t="shared" si="8"/>
         <v>0.93808630393996262</v>
       </c>
-      <c r="L11" s="13">
+      <c r="L11" s="12">
         <f t="shared" si="9"/>
         <v>3.6585365853658541E-2</v>
       </c>
-      <c r="M11" s="13">
+      <c r="M11" s="12">
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="N11" s="4"/>
-      <c r="O11" s="15">
+      <c r="O11" s="14">
         <f t="shared" si="11"/>
         <v>0</v>
       </c>
-      <c r="P11" s="16">
+      <c r="P11" s="15">
         <f t="shared" si="3"/>
         <v>2.532833020637899E-2</v>
       </c>
-      <c r="Q11" s="16">
+      <c r="Q11" s="15">
         <f t="shared" si="3"/>
         <v>0.93808630393996262</v>
       </c>
-      <c r="R11" s="16">
+      <c r="R11" s="15">
         <f t="shared" si="3"/>
         <v>3.6585365853658541E-2</v>
       </c>
-      <c r="S11" s="15">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="V11" s="15">
+      <c r="S11" s="14">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="V11" s="14">
         <v>7</v>
       </c>
       <c r="W11" s="2"/>
@@ -1395,69 +1395,69 @@
       <c r="AG11" s="2"/>
     </row>
     <row r="12" spans="1:33" x14ac:dyDescent="0.3">
-      <c r="A12" s="18" t="s">
+      <c r="A12" s="17" t="s">
         <v>29</v>
       </c>
-      <c r="B12" s="19">
+      <c r="B12" s="18">
         <v>130.14114499999999</v>
       </c>
       <c r="C12" s="8">
         <v>0</v>
       </c>
-      <c r="D12" s="13">
+      <c r="D12" s="12">
         <v>1.7000000000000001E-2</v>
       </c>
-      <c r="E12" s="14">
+      <c r="E12" s="13">
         <v>1</v>
       </c>
-      <c r="F12" s="13">
+      <c r="F12" s="12">
         <v>2.7E-2</v>
       </c>
       <c r="G12" s="8">
         <v>0</v>
       </c>
-      <c r="I12" s="13">
+      <c r="I12" s="12">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
-      <c r="J12" s="13">
+      <c r="J12" s="12">
         <f t="shared" si="7"/>
         <v>1.6283524904214565E-2</v>
       </c>
-      <c r="K12" s="13">
+      <c r="K12" s="12">
         <f t="shared" si="8"/>
         <v>0.9578544061302684</v>
       </c>
-      <c r="L12" s="13">
+      <c r="L12" s="12">
         <f t="shared" si="9"/>
         <v>2.5862068965517244E-2</v>
       </c>
-      <c r="M12" s="13">
+      <c r="M12" s="12">
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="N12" s="4"/>
-      <c r="O12" s="15">
+      <c r="O12" s="14">
         <f t="shared" si="11"/>
         <v>0</v>
       </c>
-      <c r="P12" s="16">
+      <c r="P12" s="15">
         <f t="shared" si="3"/>
         <v>1.6283524904214565E-2</v>
       </c>
-      <c r="Q12" s="16">
+      <c r="Q12" s="15">
         <f t="shared" si="3"/>
         <v>0.9578544061302684</v>
       </c>
-      <c r="R12" s="16">
+      <c r="R12" s="15">
         <f t="shared" si="3"/>
         <v>2.5862068965517244E-2</v>
       </c>
-      <c r="S12" s="15">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="V12" s="15">
+      <c r="S12" s="14">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="V12" s="14">
         <v>8</v>
       </c>
       <c r="W12" s="2"/>
@@ -1485,69 +1485,69 @@
       </c>
     </row>
     <row r="13" spans="1:33" x14ac:dyDescent="0.3">
-      <c r="A13" s="18" t="s">
+      <c r="A13" s="17" t="s">
         <v>30</v>
       </c>
-      <c r="B13" s="19">
+      <c r="B13" s="18">
         <v>131.13818000000001</v>
       </c>
       <c r="C13" s="8">
         <v>0</v>
       </c>
-      <c r="D13" s="13">
+      <c r="D13" s="12">
         <v>3.9E-2</v>
       </c>
-      <c r="E13" s="14">
+      <c r="E13" s="13">
         <v>1</v>
       </c>
-      <c r="F13" s="13">
+      <c r="F13" s="12">
         <v>3.6999999999999998E-2</v>
       </c>
       <c r="G13" s="8">
         <v>0</v>
       </c>
-      <c r="I13" s="13">
+      <c r="I13" s="12">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
-      <c r="J13" s="13">
+      <c r="J13" s="12">
         <f t="shared" si="7"/>
         <v>3.6245353159851307E-2</v>
       </c>
-      <c r="K13" s="13">
+      <c r="K13" s="12">
         <f t="shared" si="8"/>
         <v>0.92936802973977706</v>
       </c>
-      <c r="L13" s="13">
+      <c r="L13" s="12">
         <f t="shared" si="9"/>
         <v>3.4386617100371754E-2</v>
       </c>
-      <c r="M13" s="13">
+      <c r="M13" s="12">
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="N13" s="4"/>
-      <c r="O13" s="15">
+      <c r="O13" s="14">
         <f t="shared" si="11"/>
         <v>0</v>
       </c>
-      <c r="P13" s="16">
+      <c r="P13" s="15">
         <f t="shared" si="3"/>
         <v>3.6245353159851307E-2</v>
       </c>
-      <c r="Q13" s="16">
+      <c r="Q13" s="15">
         <f t="shared" si="3"/>
         <v>0.92936802973977706</v>
       </c>
-      <c r="R13" s="16">
+      <c r="R13" s="15">
         <f t="shared" si="3"/>
         <v>3.4386617100371754E-2</v>
       </c>
-      <c r="S13" s="15">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="V13" s="15">
+      <c r="S13" s="14">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="V13" s="14">
         <v>9</v>
       </c>
       <c r="W13" s="2"/>
@@ -1572,69 +1572,69 @@
       <c r="AG13" s="2"/>
     </row>
     <row r="14" spans="1:33" x14ac:dyDescent="0.3">
-      <c r="A14" s="18" t="s">
+      <c r="A14" s="17" t="s">
         <v>31</v>
       </c>
-      <c r="B14" s="19">
+      <c r="B14" s="18">
         <v>131.144499</v>
       </c>
       <c r="C14" s="8">
         <v>0</v>
       </c>
-      <c r="D14" s="13">
+      <c r="D14" s="12">
         <v>3.6999999999999998E-2</v>
       </c>
-      <c r="E14" s="14">
+      <c r="E14" s="13">
         <v>1</v>
       </c>
-      <c r="F14" s="13">
+      <c r="F14" s="12">
         <v>2.9000000000000001E-2</v>
       </c>
       <c r="G14" s="8">
         <v>0</v>
       </c>
-      <c r="I14" s="13">
+      <c r="I14" s="12">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
-      <c r="J14" s="13">
+      <c r="J14" s="12">
         <f t="shared" si="7"/>
         <v>3.4709193245778612E-2</v>
       </c>
-      <c r="K14" s="13">
+      <c r="K14" s="12">
         <f t="shared" si="8"/>
         <v>0.93808630393996262</v>
       </c>
-      <c r="L14" s="13">
+      <c r="L14" s="12">
         <f t="shared" si="9"/>
         <v>2.7204502814258916E-2</v>
       </c>
-      <c r="M14" s="13">
+      <c r="M14" s="12">
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="N14" s="4"/>
-      <c r="O14" s="15">
+      <c r="O14" s="14">
         <f t="shared" si="11"/>
         <v>0</v>
       </c>
-      <c r="P14" s="16">
+      <c r="P14" s="15">
         <f t="shared" si="3"/>
         <v>3.4709193245778612E-2</v>
       </c>
-      <c r="Q14" s="16">
+      <c r="Q14" s="15">
         <f t="shared" si="3"/>
         <v>0.93808630393996262</v>
       </c>
-      <c r="R14" s="16">
+      <c r="R14" s="15">
         <f t="shared" si="3"/>
         <v>2.7204502814258916E-2</v>
       </c>
-      <c r="S14" s="15">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="V14" s="15">
+      <c r="S14" s="14">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="V14" s="14">
         <v>10</v>
       </c>
       <c r="AC14" s="2">
@@ -1667,13 +1667,13 @@
       <c r="G16" s="8"/>
       <c r="H16" s="9"/>
       <c r="I16" s="9"/>
-      <c r="O16" s="10" t="s">
+      <c r="O16" s="19" t="s">
         <v>3</v>
       </c>
-      <c r="P16" s="10"/>
-      <c r="Q16" s="10"/>
-      <c r="R16" s="10"/>
-      <c r="S16" s="10"/>
+      <c r="P16" s="19"/>
+      <c r="Q16" s="19"/>
+      <c r="R16" s="19"/>
+      <c r="S16" s="19"/>
       <c r="T16" t="s">
         <v>32</v>
       </c>
@@ -1682,7 +1682,7 @@
       </c>
     </row>
     <row r="17" spans="4:33" x14ac:dyDescent="0.3">
-      <c r="D17" s="18"/>
+      <c r="D17" s="17"/>
       <c r="F17" s="8"/>
       <c r="G17" s="8"/>
       <c r="H17" s="8"/>
@@ -1717,7 +1717,7 @@
       <c r="U17" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="V17" s="15">
+      <c r="V17" s="14">
         <v>0</v>
       </c>
       <c r="W17">
@@ -1755,7 +1755,7 @@
       </c>
     </row>
     <row r="18" spans="4:33" x14ac:dyDescent="0.3">
-      <c r="D18" s="18"/>
+      <c r="D18" s="17"/>
       <c r="F18" s="8"/>
       <c r="G18" s="8"/>
       <c r="H18" s="8"/>
@@ -1790,7 +1790,7 @@
       <c r="U18" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="V18" s="15">
+      <c r="V18" s="14">
         <v>1</v>
       </c>
       <c r="W18">
@@ -1828,7 +1828,7 @@
       </c>
     </row>
     <row r="19" spans="4:33" x14ac:dyDescent="0.3">
-      <c r="D19" s="18"/>
+      <c r="D19" s="17"/>
       <c r="F19" s="8"/>
       <c r="G19" s="8"/>
       <c r="H19" s="8"/>
@@ -1863,7 +1863,7 @@
       <c r="U19" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="V19" s="15">
+      <c r="V19" s="14">
         <v>2</v>
       </c>
       <c r="W19">
@@ -1901,7 +1901,7 @@
       </c>
     </row>
     <row r="20" spans="4:33" x14ac:dyDescent="0.3">
-      <c r="D20" s="18"/>
+      <c r="D20" s="17"/>
       <c r="F20" s="8"/>
       <c r="G20" s="8"/>
       <c r="H20" s="8"/>
@@ -1936,7 +1936,7 @@
       <c r="U20" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="V20" s="15">
+      <c r="V20" s="14">
         <v>3</v>
       </c>
       <c r="W20">
@@ -1974,7 +1974,7 @@
       </c>
     </row>
     <row r="21" spans="4:33" x14ac:dyDescent="0.3">
-      <c r="D21" s="18"/>
+      <c r="D21" s="17"/>
       <c r="F21" s="8"/>
       <c r="G21" s="8"/>
       <c r="H21" s="8"/>
@@ -2009,7 +2009,7 @@
       <c r="U21" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="V21" s="15">
+      <c r="V21" s="14">
         <v>4</v>
       </c>
       <c r="W21">
@@ -2018,7 +2018,7 @@
       <c r="X21">
         <v>0</v>
       </c>
-      <c r="Y21" s="17">
+      <c r="Y21" s="16">
         <v>5.8999999999999997E-2</v>
       </c>
       <c r="Z21">
@@ -2047,7 +2047,7 @@
       </c>
     </row>
     <row r="22" spans="4:33" x14ac:dyDescent="0.3">
-      <c r="D22" s="18"/>
+      <c r="D22" s="17"/>
       <c r="F22" s="8"/>
       <c r="G22" s="8"/>
       <c r="H22" s="8"/>
@@ -2082,7 +2082,7 @@
       <c r="U22" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="V22" s="15">
+      <c r="V22" s="14">
         <v>5</v>
       </c>
       <c r="W22">
@@ -2120,7 +2120,7 @@
       </c>
     </row>
     <row r="23" spans="4:33" x14ac:dyDescent="0.3">
-      <c r="D23" s="18"/>
+      <c r="D23" s="17"/>
       <c r="F23" s="8"/>
       <c r="G23" s="8"/>
       <c r="H23" s="8"/>
@@ -2155,7 +2155,7 @@
       <c r="U23" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="V23" s="15">
+      <c r="V23" s="14">
         <v>6</v>
       </c>
       <c r="W23">
@@ -2193,7 +2193,7 @@
       </c>
     </row>
     <row r="24" spans="4:33" x14ac:dyDescent="0.3">
-      <c r="D24" s="18"/>
+      <c r="D24" s="17"/>
       <c r="F24" s="8"/>
       <c r="G24" s="8"/>
       <c r="H24" s="8"/>
@@ -2228,7 +2228,7 @@
       <c r="U24" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="V24" s="15">
+      <c r="V24" s="14">
         <v>7</v>
       </c>
       <c r="W24">
@@ -2266,7 +2266,7 @@
       </c>
     </row>
     <row r="25" spans="4:33" x14ac:dyDescent="0.3">
-      <c r="D25" s="18"/>
+      <c r="D25" s="17"/>
       <c r="F25" s="8"/>
       <c r="G25" s="8"/>
       <c r="H25" s="8"/>
@@ -2301,7 +2301,7 @@
       <c r="U25" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="V25" s="15">
+      <c r="V25" s="14">
         <v>8</v>
       </c>
       <c r="W25">
@@ -2339,7 +2339,7 @@
       </c>
     </row>
     <row r="26" spans="4:33" x14ac:dyDescent="0.3">
-      <c r="D26" s="18"/>
+      <c r="D26" s="17"/>
       <c r="F26" s="8"/>
       <c r="G26" s="8"/>
       <c r="H26" s="8"/>
@@ -2374,7 +2374,7 @@
       <c r="U26" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="V26" s="15">
+      <c r="V26" s="14">
         <v>9</v>
       </c>
       <c r="W26">
@@ -2412,7 +2412,7 @@
       </c>
     </row>
     <row r="27" spans="4:33" x14ac:dyDescent="0.3">
-      <c r="D27" s="18"/>
+      <c r="D27" s="17"/>
       <c r="F27" s="8"/>
       <c r="G27" s="8"/>
       <c r="H27" s="8"/>
@@ -2447,7 +2447,7 @@
       <c r="U27" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="V27" s="15">
+      <c r="V27" s="14">
         <v>10</v>
       </c>
       <c r="W27">
@@ -3023,13 +3023,13 @@
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A1" s="10" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="10"/>
-      <c r="C1" s="10"/>
-      <c r="D1" s="10"/>
-      <c r="E1" s="10"/>
+      <c r="A1" s="19" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="19"/>
+      <c r="C1" s="19"/>
+      <c r="D1" s="19"/>
+      <c r="E1" s="19"/>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A2" s="8">
@@ -3071,23 +3071,23 @@
         <f>SUM(A3:E3)</f>
         <v>1.0860000000000001</v>
       </c>
-      <c r="H3" s="12">
+      <c r="H3" s="11">
         <f>A3/$F3</f>
         <v>0</v>
       </c>
-      <c r="I3" s="12">
+      <c r="I3" s="11">
         <f t="shared" ref="I3:L3" si="0">B3/$F3</f>
         <v>0</v>
       </c>
-      <c r="J3" s="11">
+      <c r="J3" s="10">
         <f t="shared" si="0"/>
         <v>0.92081031307550643</v>
       </c>
-      <c r="K3" s="12">
+      <c r="K3" s="11">
         <f t="shared" si="0"/>
         <v>7.550644567219153E-2</v>
       </c>
-      <c r="L3" s="12">
+      <c r="L3" s="11">
         <f t="shared" si="0"/>
         <v>3.6832412523020255E-3</v>
       </c>
@@ -3112,24 +3112,24 @@
         <f t="shared" ref="F4:F13" si="1">SUM(A4:E4)</f>
         <v>1.0799999999999998</v>
       </c>
-      <c r="H4" s="12">
-        <f t="shared" ref="H4:H14" si="2">A4/$F4</f>
-        <v>0</v>
-      </c>
-      <c r="I4" s="12">
-        <f t="shared" ref="I4:I14" si="3">B4/$F4</f>
+      <c r="H4" s="11">
+        <f t="shared" ref="H4:H13" si="2">A4/$F4</f>
+        <v>0</v>
+      </c>
+      <c r="I4" s="11">
+        <f t="shared" ref="I4:I13" si="3">B4/$F4</f>
         <v>9.2592592592592607E-4</v>
       </c>
-      <c r="J4" s="11">
-        <f t="shared" ref="J4:J14" si="4">C4/$F4</f>
+      <c r="J4" s="10">
+        <f t="shared" ref="J4:J13" si="4">C4/$F4</f>
         <v>0.92592592592592604</v>
       </c>
-      <c r="K4" s="12">
-        <f t="shared" ref="K4:K14" si="5">D4/$F4</f>
+      <c r="K4" s="11">
+        <f t="shared" ref="K4:K13" si="5">D4/$F4</f>
         <v>7.3148148148148157E-2</v>
       </c>
-      <c r="L4" s="12">
-        <f t="shared" ref="L4:L14" si="6">E4/$F4</f>
+      <c r="L4" s="11">
+        <f t="shared" ref="L4:L13" si="6">E4/$F4</f>
         <v>0</v>
       </c>
     </row>
@@ -3153,23 +3153,23 @@
         <f t="shared" si="1"/>
         <v>1.0679999999999998</v>
       </c>
-      <c r="H5" s="12">
+      <c r="H5" s="11">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="I5" s="12">
+      <c r="I5" s="11">
         <f t="shared" si="3"/>
         <v>4.6816479400749074E-3</v>
       </c>
-      <c r="J5" s="11">
+      <c r="J5" s="10">
         <f t="shared" si="4"/>
         <v>0.93632958801498145</v>
       </c>
-      <c r="K5" s="12">
+      <c r="K5" s="11">
         <f t="shared" si="5"/>
         <v>5.8988764044943832E-2</v>
       </c>
-      <c r="L5" s="12">
+      <c r="L5" s="11">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
@@ -3194,23 +3194,23 @@
         <f t="shared" si="1"/>
         <v>1.0639999999999998</v>
       </c>
-      <c r="H6" s="12">
+      <c r="H6" s="11">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="I6" s="12">
+      <c r="I6" s="11">
         <f t="shared" si="3"/>
         <v>6.578947368421054E-3</v>
       </c>
-      <c r="J6" s="11">
+      <c r="J6" s="10">
         <f t="shared" si="4"/>
         <v>0.93984962406015049</v>
       </c>
-      <c r="K6" s="12">
+      <c r="K6" s="11">
         <f t="shared" si="5"/>
         <v>5.3571428571428582E-2</v>
       </c>
-      <c r="L6" s="12">
+      <c r="L6" s="11">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
@@ -3235,23 +3235,23 @@
         <f t="shared" si="1"/>
         <v>1.0780000000000001</v>
       </c>
-      <c r="H7" s="12">
+      <c r="H7" s="11">
         <f t="shared" si="2"/>
         <v>1.8552875695732837E-3</v>
       </c>
-      <c r="I7" s="12">
+      <c r="I7" s="11">
         <f t="shared" si="3"/>
         <v>1.4842300556586269E-2</v>
       </c>
-      <c r="J7" s="11">
+      <c r="J7" s="10">
         <f t="shared" si="4"/>
         <v>0.92764378478664189</v>
       </c>
-      <c r="K7" s="12">
+      <c r="K7" s="11">
         <f t="shared" si="5"/>
         <v>5.5658627087198508E-2</v>
       </c>
-      <c r="L7" s="12">
+      <c r="L7" s="11">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
@@ -3276,23 +3276,23 @@
         <f t="shared" si="1"/>
         <v>1.075</v>
       </c>
-      <c r="H8" s="12">
+      <c r="H8" s="11">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="I8" s="12">
+      <c r="I8" s="11">
         <f t="shared" si="3"/>
         <v>2.3255813953488375E-2</v>
       </c>
-      <c r="J8" s="11">
+      <c r="J8" s="10">
         <f t="shared" si="4"/>
         <v>0.93023255813953487</v>
       </c>
-      <c r="K8" s="12">
+      <c r="K8" s="11">
         <f t="shared" si="5"/>
         <v>4.651162790697675E-2</v>
       </c>
-      <c r="L8" s="12">
+      <c r="L8" s="11">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
@@ -3317,23 +3317,23 @@
         <f t="shared" si="1"/>
         <v>1.0659999999999998</v>
       </c>
-      <c r="H9" s="12">
+      <c r="H9" s="11">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="I9" s="12">
+      <c r="I9" s="11">
         <f t="shared" si="3"/>
         <v>2.1575984990619138E-2</v>
       </c>
-      <c r="J9" s="11">
+      <c r="J9" s="10">
         <f t="shared" si="4"/>
         <v>0.93808630393996262</v>
       </c>
-      <c r="K9" s="12">
+      <c r="K9" s="11">
         <f t="shared" si="5"/>
         <v>4.0337711069418386E-2</v>
       </c>
-      <c r="L9" s="12">
+      <c r="L9" s="11">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
@@ -3358,23 +3358,23 @@
         <f t="shared" si="1"/>
         <v>1.0659999999999998</v>
       </c>
-      <c r="H10" s="12">
+      <c r="H10" s="11">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="I10" s="12">
+      <c r="I10" s="11">
         <f t="shared" si="3"/>
         <v>2.532833020637899E-2</v>
       </c>
-      <c r="J10" s="11">
+      <c r="J10" s="10">
         <f t="shared" si="4"/>
         <v>0.93808630393996262</v>
       </c>
-      <c r="K10" s="12">
+      <c r="K10" s="11">
         <f t="shared" si="5"/>
         <v>3.6585365853658541E-2</v>
       </c>
-      <c r="L10" s="12">
+      <c r="L10" s="11">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
@@ -3399,23 +3399,23 @@
         <f t="shared" si="1"/>
         <v>1.0439999999999998</v>
       </c>
-      <c r="H11" s="12">
+      <c r="H11" s="11">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="I11" s="12">
+      <c r="I11" s="11">
         <f t="shared" si="3"/>
         <v>1.6283524904214565E-2</v>
       </c>
-      <c r="J11" s="11">
+      <c r="J11" s="10">
         <f t="shared" si="4"/>
         <v>0.9578544061302684</v>
       </c>
-      <c r="K11" s="12">
+      <c r="K11" s="11">
         <f t="shared" si="5"/>
         <v>2.5862068965517244E-2</v>
       </c>
-      <c r="L11" s="12">
+      <c r="L11" s="11">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
@@ -3440,23 +3440,23 @@
         <f t="shared" si="1"/>
         <v>1.0759999999999998</v>
       </c>
-      <c r="H12" s="12">
+      <c r="H12" s="11">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="I12" s="12">
+      <c r="I12" s="11">
         <f t="shared" si="3"/>
         <v>3.6245353159851307E-2</v>
       </c>
-      <c r="J12" s="11">
+      <c r="J12" s="10">
         <f t="shared" si="4"/>
         <v>0.92936802973977706</v>
       </c>
-      <c r="K12" s="12">
+      <c r="K12" s="11">
         <f t="shared" si="5"/>
         <v>3.4386617100371754E-2</v>
       </c>
-      <c r="L12" s="12">
+      <c r="L12" s="11">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
@@ -3481,79 +3481,79 @@
         <f t="shared" si="1"/>
         <v>1.0659999999999998</v>
       </c>
-      <c r="H13" s="12">
+      <c r="H13" s="11">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="I13" s="12">
+      <c r="I13" s="11">
         <f t="shared" si="3"/>
         <v>3.4709193245778612E-2</v>
       </c>
-      <c r="J13" s="11">
+      <c r="J13" s="10">
         <f t="shared" si="4"/>
         <v>0.93808630393996262</v>
       </c>
-      <c r="K13" s="12">
+      <c r="K13" s="11">
         <f t="shared" si="5"/>
         <v>2.7204502814258916E-2</v>
       </c>
-      <c r="L13" s="12">
+      <c r="L13" s="11">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="J16" s="11">
+      <c r="J16" s="10">
         <v>0.91400000000000003</v>
       </c>
     </row>
     <row r="17" spans="10:10" x14ac:dyDescent="0.3">
-      <c r="J17" s="11">
+      <c r="J17" s="10">
         <v>0.92</v>
       </c>
     </row>
     <row r="18" spans="10:10" x14ac:dyDescent="0.3">
-      <c r="J18" s="11">
+      <c r="J18" s="10">
         <v>0.93200000000000005</v>
       </c>
     </row>
     <row r="19" spans="10:10" x14ac:dyDescent="0.3">
-      <c r="J19" s="11">
+      <c r="J19" s="10">
         <v>0.93599999999999994</v>
       </c>
     </row>
     <row r="20" spans="10:10" x14ac:dyDescent="0.3">
-      <c r="J20" s="11">
+      <c r="J20" s="10">
         <v>0.92199999999999993</v>
       </c>
     </row>
     <row r="21" spans="10:10" x14ac:dyDescent="0.3">
-      <c r="J21" s="11">
+      <c r="J21" s="10">
         <v>0.92499999999999993</v>
       </c>
     </row>
     <row r="22" spans="10:10" x14ac:dyDescent="0.3">
-      <c r="J22" s="11">
+      <c r="J22" s="10">
         <v>0.93399999999999994</v>
       </c>
     </row>
     <row r="23" spans="10:10" x14ac:dyDescent="0.3">
-      <c r="J23" s="11">
+      <c r="J23" s="10">
         <v>0.93399999999999994</v>
       </c>
     </row>
     <row r="24" spans="10:10" x14ac:dyDescent="0.3">
-      <c r="J24" s="11">
+      <c r="J24" s="10">
         <v>0.95599999999999996</v>
       </c>
     </row>
     <row r="25" spans="10:10" x14ac:dyDescent="0.3">
-      <c r="J25" s="11">
+      <c r="J25" s="10">
         <v>0.92399999999999993</v>
       </c>
     </row>
     <row r="26" spans="10:10" x14ac:dyDescent="0.3">
-      <c r="J26" s="11">
+      <c r="J26" s="10">
         <v>0.93399999999999994</v>
       </c>
     </row>

</xml_diff>